<commit_message>
Merch Conflicts in Login, PDP and Registration.
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="230430" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="6" activeTab="10"/>
+    <workbookView xWindow="230430" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="SetupBrowsers" sheetId="50" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5204" uniqueCount="988">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5213" uniqueCount="988">
   <si>
     <t>Please enter a valid email</t>
   </si>
@@ -4242,7 +4242,7 @@
   </sheetPr>
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -5001,8 +5001,8 @@
   </sheetPr>
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16905,7 +16905,7 @@
   <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView topLeftCell="A37" zoomScale="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B46"/>
+      <selection activeCell="K46" sqref="A46:K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18418,8 +18418,8 @@
   </sheetPr>
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A34" zoomScale="85" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19743,10 +19743,10 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B40"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21055,6 +21055,37 @@
       <c r="K40" s="117" t="s">
         <v>514</v>
       </c>
+    </row>
+    <row r="41" spans="1:11" ht="75">
+      <c r="A41" s="95" t="s">
+        <v>728</v>
+      </c>
+      <c r="B41" s="95" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="130" t="s">
+        <v>983</v>
+      </c>
+      <c r="D41" s="130" t="s">
+        <v>980</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>975</v>
+      </c>
+      <c r="F41" s="130" t="s">
+        <v>972</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="J41" s="87"/>
+      <c r="K41" s="128"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>